<commit_message>
all figures and tables updated
</commit_message>
<xml_diff>
--- a/comparison-scripts/2009_supp_tables.xlsx
+++ b/comparison-scripts/2009_supp_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppf6\Desktop\GitHub\FluCode\comparison-scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{32E89272-6FC5-4438-B49B-6AE9EDF38163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C591AE-A449-4017-843D-3CE5CC83D758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="perc ill" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1262,15 +1262,6 @@
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1312,6 +1303,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1329,33 +1356,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1711,7 +1711,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1727,246 +1727,246 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="4"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1981,7 +1981,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2233,7 +2233,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2489,11 +2489,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2506,129 +2506,129 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
-      <c r="J2" s="18"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="J3" s="18"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="4"/>
-      <c r="C4" s="25" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="18" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D11" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E11" s="24" t="s">
         <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>